<commit_message>
sửa nốt class, menu sidebar, kích thước bảng
</commit_message>
<xml_diff>
--- a/Class_Stats_Report_2025-2026.xlsx
+++ b/Class_Stats_Report_2025-2026.xlsx
@@ -28,25 +28,25 @@
     <t>Đánh giá và kiểm định</t>
   </si>
   <si>
+    <t>Cơ sở dữ liệu</t>
+  </si>
+  <si>
     <t>Toán rời rạc</t>
   </si>
   <si>
     <t>Lập trình Python</t>
   </si>
   <si>
-    <t>Cơ sở dữ liệu</t>
-  </si>
-  <si>
     <t>250</t>
   </si>
   <si>
+    <t>430</t>
+  </si>
+  <si>
     <t>120</t>
   </si>
   <si>
-    <t>305</t>
-  </si>
-  <si>
-    <t>210</t>
+    <t>275</t>
   </si>
 </sst>
 </file>
@@ -437,7 +437,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -448,7 +448,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -459,7 +459,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
update UC 2 UC1 còn có lỗi (sql chưa chắc đúng)
</commit_message>
<xml_diff>
--- a/Class_Stats_Report_2025-2026.xlsx
+++ b/Class_Stats_Report_2025-2026.xlsx
@@ -13,56 +13,10 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Module</t>
-  </si>
-  <si>
-    <t>Num Classes</t>
-  </si>
-  <si>
-    <t>Total Students</t>
-  </si>
-  <si>
-    <t>Đánh giá và kiểm định</t>
-  </si>
-  <si>
-    <t>Cơ sở dữ liệu</t>
-  </si>
-  <si>
-    <t>Toán rời rạc</t>
-  </si>
-  <si>
-    <t>Lập trình Python</t>
-  </si>
-  <si>
-    <t>250</t>
-  </si>
-  <si>
-    <t>430</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>275</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -78,7 +32,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -86,30 +40,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,68 +340,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>